<commit_message>
feat(hyd): Actuator position control (#6155)
* Internal improvements for future actuator implementations
</commit_message>
<xml_diff>
--- a/src/systems/systems/src/hydraulic/study/Docs/Knowledge_Data_Base.xlsx
+++ b/src/systems/systems/src/hydraulic/study/Docs/Knowledge_Data_Base.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davy\Documents\A320 simulator\Hydraulics\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F70C1-8EF9-4877-8A3E-FB95F472C6D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F7F1702-2DC5-46C0-945F-5090C0C639AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{840DC6BD-CADF-4DA5-B109-8F62026FFD29}"/>
   </bookViews>
@@ -41,9 +41,27 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={D01A08D8-CFE0-40E4-8767-ED551164DBCA}</author>
+    <author>tc={6BF4E57B-D71C-495E-B998-88CA71A02042}</author>
+    <author>tc={D0411326-7E73-41E5-B4A5-1F9987989333}</author>
   </authors>
   <commentList>
     <comment ref="D33" authorId="0" shapeId="0" xr:uid="{D01A08D8-CFE0-40E4-8767-ED551164DBCA}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    This value gives correct actuator displacement</t>
+      </text>
+    </comment>
+    <comment ref="D40" authorId="1" shapeId="0" xr:uid="{6BF4E57B-D71C-495E-B998-88CA71A02042}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    This value gives correct actuator displacement</t>
+      </text>
+    </comment>
+    <comment ref="D47" authorId="2" shapeId="0" xr:uid="{D0411326-7E73-41E5-B4A5-1F9987989333}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>Aileron</t>
   </si>
@@ -275,13 +293,19 @@
   </si>
   <si>
     <t>Max Rated Speed : 7600 RPM</t>
+  </si>
+  <si>
+    <t>Both actuators</t>
+  </si>
+  <si>
+    <t>Main gear door</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +384,12 @@
       <sz val="6"/>
       <color rgb="FF000000"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -509,7 +539,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>609730</xdr:colOff>
+      <xdr:colOff>609731</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>99702</xdr:rowOff>
     </xdr:to>
@@ -540,6 +570,67 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>344976</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>140074</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1202953</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>52668</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF420DB1-EEEC-438C-A958-2B0827C097B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8407609" y="8387603"/>
+          <a:ext cx="5054579" cy="5470712"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1107,6 +1198,12 @@
   <threadedComment ref="D33" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{D01A08D8-CFE0-40E4-8767-ED551164DBCA}">
     <text>This value gives correct actuator displacement</text>
   </threadedComment>
+  <threadedComment ref="D40" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{6BF4E57B-D71C-495E-B998-88CA71A02042}">
+    <text>This value gives correct actuator displacement</text>
+  </threadedComment>
+  <threadedComment ref="D47" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{D0411326-7E73-41E5-B4A5-1F9987989333}">
+    <text>This value gives correct actuator displacement</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1115,7 +1212,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1247,14 +1344,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115B7D6A-2F7B-4E42-B420-A9A26CD5C1D2}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
     <col min="2" max="2" width="20.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -1445,7 +1543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="3:6">
+    <row r="33" spans="1:10">
       <c r="C33" s="4">
         <v>-0.1</v>
       </c>
@@ -1459,25 +1557,251 @@
         <v>0.18149999999999999</v>
       </c>
     </row>
-    <row r="38" spans="3:6">
-      <c r="D38">
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6">
-      <c r="D39">
-        <f>D38*6894.76</f>
-        <v>8652923.8000000007</v>
-      </c>
-      <c r="E39">
-        <f>D39*E30</f>
-        <v>143432.14279605995</v>
+    <row r="36" spans="1:10">
+      <c r="B36" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4.4220000000000002E-2</v>
+      </c>
+      <c r="D37" s="2">
+        <f>2*SQRT(0.00089/PI())</f>
+        <v>3.3662786498064812E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <f>PI()* (C37/2)^2</f>
+        <v>1.535774166051943E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>PI()* (D37/2)^2</f>
+        <v>8.8999999999999973E-4</v>
+      </c>
+      <c r="G37" s="1">
+        <f>E37*B37</f>
+        <v>5.5902179644290722E-4</v>
+      </c>
+      <c r="H37" s="1">
+        <f>(E37-F37)*B37</f>
+        <v>2.3506179644290734E-4</v>
+      </c>
+      <c r="I37" s="1">
+        <f>G37/H37</f>
+        <v>2.3781907774991606</v>
+      </c>
+      <c r="J37" s="1">
+        <f>(G37-H37) * 1000</f>
+        <v>0.32395999999999986</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38">
+        <f>G37*2</f>
+        <v>1.1180435928858144E-3</v>
+      </c>
+      <c r="H38">
+        <f>H37*2</f>
+        <v>4.7012359288581469E-4</v>
+      </c>
+      <c r="I38">
+        <f>G38/H38</f>
+        <v>2.3781907774991606</v>
+      </c>
+      <c r="J38" s="1">
+        <f>(G38-H38) * 1000</f>
+        <v>0.64791999999999972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="B39" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="C40" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="E40" s="4">
+        <v>-0.76500000000000001</v>
+      </c>
+      <c r="F40" s="3">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="B43" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="C44" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D44" s="2">
+        <f>0.03</f>
+        <v>0.03</v>
+      </c>
+      <c r="E44" s="1">
+        <f>PI()* (C44/2)^2</f>
+        <v>2.3758294442772811E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>PI()* (D44/2)^2</f>
+        <v>7.0685834705770342E-4</v>
+      </c>
+      <c r="G44" s="1">
+        <f>E44*B44</f>
+        <v>9.0281518882536686E-4</v>
+      </c>
+      <c r="H44" s="1">
+        <f>(E44-F44)*B44</f>
+        <v>6.3420901694343954E-4</v>
+      </c>
+      <c r="I44" s="1">
+        <f>G44/H44</f>
+        <v>1.4235294117647059</v>
+      </c>
+      <c r="J44" s="1">
+        <f>(G44-H44) * 1000</f>
+        <v>0.26860617188192731</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45">
+        <f>G44*2</f>
+        <v>1.8056303776507337E-3</v>
+      </c>
+      <c r="H45">
+        <f>H44*2</f>
+        <v>1.2684180338868791E-3</v>
+      </c>
+      <c r="I45">
+        <f>G45/H45</f>
+        <v>1.4235294117647059</v>
+      </c>
+      <c r="J45" s="1">
+        <f>(G45-H45) * 1000</f>
+        <v>0.53721234376385463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="B46" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="C47" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1492,7 +1816,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17.06640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.06640625" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1639,11 +1963,11 @@
         <v>9</v>
       </c>
       <c r="D14">
-        <f>B14*0.264172/60</f>
+        <f t="shared" ref="D14:E16" si="0">B14*0.264172/60</f>
         <v>3.1700640000000002E-2</v>
       </c>
       <c r="E14">
-        <f>C14*0.264172/60</f>
+        <f t="shared" si="0"/>
         <v>3.9625800000000003E-2</v>
       </c>
     </row>
@@ -1658,11 +1982,11 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <f>B15*0.264172/60</f>
+        <f t="shared" si="0"/>
         <v>3.1700640000000002E-2</v>
       </c>
       <c r="E15">
-        <f>C15*0.264172/60</f>
+        <f t="shared" si="0"/>
         <v>4.4028666666666674E-2</v>
       </c>
     </row>
@@ -1677,11 +2001,11 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <f>B16*0.264172/60</f>
+        <f t="shared" si="0"/>
         <v>3.3021500000000002E-2</v>
       </c>
       <c r="E16">
-        <f>C16*0.264172/60</f>
+        <f t="shared" si="0"/>
         <v>4.4028666666666674E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated gear actuators data
</commit_message>
<xml_diff>
--- a/src/systems/systems/src/hydraulic/study/Docs/Knowledge_Data_Base.xlsx
+++ b/src/systems/systems/src/hydraulic/study/Docs/Knowledge_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davy\Documents\A320 simulator\Hydraulics\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davy\Documents\GitHub\a32nx\src\systems\systems\src\hydraulic\study\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F7F1702-2DC5-46C0-945F-5090C0C639AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D83C8A2-243B-41FC-9D44-D2499E8ECA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{840DC6BD-CADF-4DA5-B109-8F62026FFD29}"/>
+    <workbookView xWindow="285" yWindow="2438" windowWidth="20250" windowHeight="12435" activeTab="1" xr2:uid="{840DC6BD-CADF-4DA5-B109-8F62026FFD29}"/>
   </bookViews>
   <sheets>
     <sheet name="Moving parts" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,8 @@
     <author>tc={D01A08D8-CFE0-40E4-8767-ED551164DBCA}</author>
     <author>tc={6BF4E57B-D71C-495E-B998-88CA71A02042}</author>
     <author>tc={D0411326-7E73-41E5-B4A5-1F9987989333}</author>
+    <author>tc={A0D3FD10-31A2-424D-870F-2698B6EB431B}</author>
+    <author>tc={91C1E2F8-6858-47B5-9446-46E066F4D7B3}</author>
   </authors>
   <commentList>
     <comment ref="D33" authorId="0" shapeId="0" xr:uid="{D01A08D8-CFE0-40E4-8767-ED551164DBCA}">
@@ -69,12 +71,28 @@
     This value gives correct actuator displacement</t>
       </text>
     </comment>
+    <comment ref="D54" authorId="3" shapeId="0" xr:uid="{A0D3FD10-31A2-424D-870F-2698B6EB431B}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    This value gives correct actuator displacement</t>
+      </text>
+    </comment>
+    <comment ref="D62" authorId="4" shapeId="0" xr:uid="{91C1E2F8-6858-47B5-9446-46E066F4D7B3}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    This value gives correct actuator displacement</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
   <si>
     <t>Aileron</t>
   </si>
@@ -299,6 +317,33 @@
   </si>
   <si>
     <t>Main gear door</t>
+  </si>
+  <si>
+    <t>Nose gear door</t>
+  </si>
+  <si>
+    <t>Max force retract</t>
+  </si>
+  <si>
+    <t>Max force extend</t>
+  </si>
+  <si>
+    <t>Note those coordinates are chosen "randomly" so we get the correct actuator travel of 162mm</t>
+  </si>
+  <si>
+    <t>This actuator in fact should push a crankbell that gives a particular motion ratio.</t>
+  </si>
+  <si>
+    <t>Nose gear</t>
+  </si>
+  <si>
+    <t>Note those coordinates are chosen "randomly" so we get the correct actuator travel of 320mm</t>
+  </si>
+  <si>
+    <t>Control Arm position Z</t>
+  </si>
+  <si>
+    <t>Anchor point position Z</t>
   </si>
 </sst>
 </file>
@@ -389,7 +434,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -436,12 +481,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,16 +620,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>344976</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>140074</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1840963</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>16808</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1202953</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>52668</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>424144</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>108697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -615,7 +659,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8407609" y="8387603"/>
+          <a:off x="14100198" y="7188573"/>
           <a:ext cx="5054579" cy="5470712"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1204,6 +1248,12 @@
   <threadedComment ref="D47" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{D0411326-7E73-41E5-B4A5-1F9987989333}">
     <text>This value gives correct actuator displacement</text>
   </threadedComment>
+  <threadedComment ref="D54" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{A0D3FD10-31A2-424D-870F-2698B6EB431B}">
+    <text>This value gives correct actuator displacement</text>
+  </threadedComment>
+  <threadedComment ref="D62" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{91C1E2F8-6858-47B5-9446-46E066F4D7B3}">
+    <text>This value gives correct actuator displacement</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1344,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115B7D6A-2F7B-4E42-B420-A9A26CD5C1D2}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1365,30 +1415,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -1411,7 +1461,7 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="2"/>
@@ -1443,30 +1493,30 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -1489,7 +1539,7 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="2">
@@ -1527,44 +1577,58 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="H32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I32" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>-0.1</v>
       </c>
       <c r="D33" s="3">
         <v>0.18149999999999999</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>0.5</v>
       </c>
       <c r="F33" s="3">
         <v>0.18149999999999999</v>
       </c>
+      <c r="H33">
+        <f>(E30-F30)*20684000</f>
+        <v>164841.18760030816</v>
+      </c>
+      <c r="I33">
+        <f>E30*20684000</f>
+        <v>342861.03866923036</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -1587,7 +1651,7 @@
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="2">
@@ -1647,44 +1711,58 @@
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="H39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>-0.1</v>
       </c>
       <c r="D40" s="3">
         <v>-0.2</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>-0.76500000000000001</v>
       </c>
       <c r="F40" s="3">
         <v>-0.2</v>
       </c>
+      <c r="H40">
+        <f>(E37-F37)*20684000</f>
+        <v>13357.192850618394</v>
+      </c>
+      <c r="I40">
+        <f>E37*20684000</f>
+        <v>31765.952850618389</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -1707,42 +1785,42 @@
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B44" s="2">
         <v>0.38</v>
       </c>
       <c r="C44" s="2">
-        <v>5.5E-2</v>
+        <v>5.3800000000000001E-2</v>
       </c>
       <c r="D44" s="2">
-        <f>0.03</f>
-        <v>0.03</v>
+        <f>0.03015</f>
+        <v>3.015E-2</v>
       </c>
       <c r="E44" s="1">
         <f>PI()* (C44/2)^2</f>
-        <v>2.3758294442772811E-3</v>
+        <v>2.2732878600641099E-3</v>
       </c>
       <c r="F44" s="1">
         <f>PI()* (D44/2)^2</f>
-        <v>7.0685834705770342E-4</v>
+        <v>7.1394460198695691E-4</v>
       </c>
       <c r="G44" s="1">
         <f>E44*B44</f>
-        <v>9.0281518882536686E-4</v>
+        <v>8.638493868243618E-4</v>
       </c>
       <c r="H44" s="1">
         <f>(E44-F44)*B44</f>
-        <v>6.3420901694343954E-4</v>
+        <v>5.9255043806931808E-4</v>
       </c>
       <c r="I44" s="1">
         <f>G44/H44</f>
-        <v>1.4235294117647059</v>
+        <v>1.4578495454986171</v>
       </c>
       <c r="J44" s="1">
         <f>(G44-H44) * 1000</f>
-        <v>0.26860617188192731</v>
+        <v>0.27129894875504373</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1751,50 +1829,347 @@
       </c>
       <c r="G45">
         <f>G44*2</f>
-        <v>1.8056303776507337E-3</v>
+        <v>1.7276987736487236E-3</v>
       </c>
       <c r="H45">
         <f>H44*2</f>
-        <v>1.2684180338868791E-3</v>
+        <v>1.1851008761386362E-3</v>
       </c>
       <c r="I45">
         <f>G45/H45</f>
-        <v>1.4235294117647059</v>
+        <v>1.4578495454986171</v>
       </c>
       <c r="J45" s="1">
         <f>(G45-H45) * 1000</f>
-        <v>0.53721234376385463</v>
+        <v>0.54259789751008747</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="H46" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="C47" s="4">
+      <c r="C47" s="3">
         <v>0.76</v>
       </c>
       <c r="D47" s="3">
         <v>0</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="3">
         <v>0.19</v>
       </c>
       <c r="F47" s="3">
         <v>0.23</v>
+      </c>
+      <c r="H47">
+        <f>(E44-F44)*20684000</f>
+        <v>32253.45595006783</v>
+      </c>
+      <c r="I47">
+        <f>E44*20684000</f>
+        <v>47020.686097566053</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="B50" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3.78E-2</v>
+      </c>
+      <c r="D51" s="2">
+        <f>0.023</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="E51" s="1">
+        <f>PI()* (C51/2)^2</f>
+        <v>1.12220831178881E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>PI()* (D51/2)^2</f>
+        <v>4.154756284372501E-4</v>
+      </c>
+      <c r="G51" s="1">
+        <f>E51*B51</f>
+        <v>1.8179774650978724E-4</v>
+      </c>
+      <c r="H51" s="1">
+        <f>(E51-F51)*B51</f>
+        <v>1.144906947029527E-4</v>
+      </c>
+      <c r="I51" s="1">
+        <f>G51/H51</f>
+        <v>1.5878822901849219</v>
+      </c>
+      <c r="J51" s="1">
+        <f>(G51-H51) * 1000</f>
+        <v>6.7307051806834536E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="G52">
+        <f>G51*2</f>
+        <v>3.6359549301957447E-4</v>
+      </c>
+      <c r="H52">
+        <f>H51*2</f>
+        <v>2.289813894059054E-4</v>
+      </c>
+      <c r="I52">
+        <f>G52/H52</f>
+        <v>1.5878822901849219</v>
+      </c>
+      <c r="J52" s="1">
+        <f>(G52-H52) * 1000</f>
+        <v>0.13461410361366907</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="B53" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" t="s">
+        <v>76</v>
+      </c>
+      <c r="I53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="C54" s="3">
+        <v>-0.14649999999999999</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>-0.14649999999999999</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H54">
+        <f>(E51-F51)*20684000</f>
+        <v>14618.058822443663</v>
+      </c>
+      <c r="I54">
+        <f>E51*20684000</f>
+        <v>23211.756721039746</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="B58" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="C59" s="2">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="D59" s="2">
+        <f>0.035</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E59" s="1">
+        <f>PI()* (C59/2)^2</f>
+        <v>4.9265199356533706E-3</v>
+      </c>
+      <c r="F59" s="1">
+        <f>PI()* (D59/2)^2</f>
+        <v>9.6211275016187424E-4</v>
+      </c>
+      <c r="G59" s="1">
+        <f>E59*B59</f>
+        <v>1.5764863794090786E-3</v>
+      </c>
+      <c r="H59" s="1">
+        <f>(E59-F59)*B59</f>
+        <v>1.2686102993572791E-3</v>
+      </c>
+      <c r="I59" s="1">
+        <f>G59/H59</f>
+        <v>1.242687671862494</v>
+      </c>
+      <c r="J59" s="1">
+        <f>(G59-H59) * 1000</f>
+        <v>0.30787608005179951</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60">
+        <f>G59*2</f>
+        <v>3.1529727588181572E-3</v>
+      </c>
+      <c r="H60">
+        <f>H59*2</f>
+        <v>2.5372205987145582E-3</v>
+      </c>
+      <c r="I60">
+        <f>G60/H60</f>
+        <v>1.242687671862494</v>
+      </c>
+      <c r="J60" s="1">
+        <f>(G60-H60) * 1000</f>
+        <v>0.61575216010359901</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="B61" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" t="s">
+        <v>76</v>
+      </c>
+      <c r="I61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="C62" s="3">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="D62" s="3">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H62">
+        <f>(E59-F59)*20684000</f>
+        <v>81999.798224706115</v>
+      </c>
+      <c r="I62">
+        <f>E59*20684000</f>
+        <v>101900.13834905432</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="C63" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2010,7 +2385,7 @@
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2039,47 +2414,47 @@
       </c>
     </row>
     <row r="35" spans="10:10" ht="15">
-      <c r="J35" s="16" t="s">
+      <c r="J35" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="36" spans="10:10">
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="10:10">
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="38" spans="10:10">
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="39" spans="10:10" ht="22.5">
-      <c r="J39" s="16" t="s">
+      <c r="J39" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="40" spans="10:10">
-      <c r="J40" s="17" t="s">
+      <c r="J40" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="41" spans="10:10" ht="15">
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="10:10">
-      <c r="J42" s="17" t="s">
+      <c r="J42" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="43" spans="10:10" ht="22.5">
-      <c r="J43" s="16" t="s">
+      <c r="J43" s="15" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(hyd): hydraulic gear system (#6893) @1b632aaf5
</commit_message>
<xml_diff>
--- a/src/systems/systems/src/hydraulic/study/Docs/Knowledge_Data_Base.xlsx
+++ b/src/systems/systems/src/hydraulic/study/Docs/Knowledge_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davy\Documents\A320 simulator\Hydraulics\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davy\Documents\GitHub\a32nx\src\systems\systems\src\hydraulic\study\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F7F1702-2DC5-46C0-945F-5090C0C639AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D83C8A2-243B-41FC-9D44-D2499E8ECA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{840DC6BD-CADF-4DA5-B109-8F62026FFD29}"/>
+    <workbookView xWindow="285" yWindow="2438" windowWidth="20250" windowHeight="12435" activeTab="1" xr2:uid="{840DC6BD-CADF-4DA5-B109-8F62026FFD29}"/>
   </bookViews>
   <sheets>
     <sheet name="Moving parts" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,8 @@
     <author>tc={D01A08D8-CFE0-40E4-8767-ED551164DBCA}</author>
     <author>tc={6BF4E57B-D71C-495E-B998-88CA71A02042}</author>
     <author>tc={D0411326-7E73-41E5-B4A5-1F9987989333}</author>
+    <author>tc={A0D3FD10-31A2-424D-870F-2698B6EB431B}</author>
+    <author>tc={91C1E2F8-6858-47B5-9446-46E066F4D7B3}</author>
   </authors>
   <commentList>
     <comment ref="D33" authorId="0" shapeId="0" xr:uid="{D01A08D8-CFE0-40E4-8767-ED551164DBCA}">
@@ -69,12 +71,28 @@
     This value gives correct actuator displacement</t>
       </text>
     </comment>
+    <comment ref="D54" authorId="3" shapeId="0" xr:uid="{A0D3FD10-31A2-424D-870F-2698B6EB431B}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    This value gives correct actuator displacement</t>
+      </text>
+    </comment>
+    <comment ref="D62" authorId="4" shapeId="0" xr:uid="{91C1E2F8-6858-47B5-9446-46E066F4D7B3}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    This value gives correct actuator displacement</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
   <si>
     <t>Aileron</t>
   </si>
@@ -299,6 +317,33 @@
   </si>
   <si>
     <t>Main gear door</t>
+  </si>
+  <si>
+    <t>Nose gear door</t>
+  </si>
+  <si>
+    <t>Max force retract</t>
+  </si>
+  <si>
+    <t>Max force extend</t>
+  </si>
+  <si>
+    <t>Note those coordinates are chosen "randomly" so we get the correct actuator travel of 162mm</t>
+  </si>
+  <si>
+    <t>This actuator in fact should push a crankbell that gives a particular motion ratio.</t>
+  </si>
+  <si>
+    <t>Nose gear</t>
+  </si>
+  <si>
+    <t>Note those coordinates are chosen "randomly" so we get the correct actuator travel of 320mm</t>
+  </si>
+  <si>
+    <t>Control Arm position Z</t>
+  </si>
+  <si>
+    <t>Anchor point position Z</t>
   </si>
 </sst>
 </file>
@@ -389,7 +434,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -436,12 +481,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,16 +620,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>344976</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>140074</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1840963</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>16808</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1202953</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>52668</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>424144</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>108697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -615,7 +659,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8407609" y="8387603"/>
+          <a:off x="14100198" y="7188573"/>
           <a:ext cx="5054579" cy="5470712"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1204,6 +1248,12 @@
   <threadedComment ref="D47" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{D0411326-7E73-41E5-B4A5-1F9987989333}">
     <text>This value gives correct actuator displacement</text>
   </threadedComment>
+  <threadedComment ref="D54" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{A0D3FD10-31A2-424D-870F-2698B6EB431B}">
+    <text>This value gives correct actuator displacement</text>
+  </threadedComment>
+  <threadedComment ref="D62" dT="2021-01-29T14:42:20.37" personId="{F15DFD44-D410-4C9C-83B2-CB0EB835C9C8}" id="{91C1E2F8-6858-47B5-9446-46E066F4D7B3}">
+    <text>This value gives correct actuator displacement</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1344,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115B7D6A-2F7B-4E42-B420-A9A26CD5C1D2}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1365,30 +1415,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -1411,7 +1461,7 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="2"/>
@@ -1443,30 +1493,30 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -1489,7 +1539,7 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="2">
@@ -1527,44 +1577,58 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="H32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I32" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>-0.1</v>
       </c>
       <c r="D33" s="3">
         <v>0.18149999999999999</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>0.5</v>
       </c>
       <c r="F33" s="3">
         <v>0.18149999999999999</v>
       </c>
+      <c r="H33">
+        <f>(E30-F30)*20684000</f>
+        <v>164841.18760030816</v>
+      </c>
+      <c r="I33">
+        <f>E30*20684000</f>
+        <v>342861.03866923036</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -1587,7 +1651,7 @@
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="2">
@@ -1647,44 +1711,58 @@
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="H39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>-0.1</v>
       </c>
       <c r="D40" s="3">
         <v>-0.2</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>-0.76500000000000001</v>
       </c>
       <c r="F40" s="3">
         <v>-0.2</v>
       </c>
+      <c r="H40">
+        <f>(E37-F37)*20684000</f>
+        <v>13357.192850618394</v>
+      </c>
+      <c r="I40">
+        <f>E37*20684000</f>
+        <v>31765.952850618389</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -1707,42 +1785,42 @@
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B44" s="2">
         <v>0.38</v>
       </c>
       <c r="C44" s="2">
-        <v>5.5E-2</v>
+        <v>5.3800000000000001E-2</v>
       </c>
       <c r="D44" s="2">
-        <f>0.03</f>
-        <v>0.03</v>
+        <f>0.03015</f>
+        <v>3.015E-2</v>
       </c>
       <c r="E44" s="1">
         <f>PI()* (C44/2)^2</f>
-        <v>2.3758294442772811E-3</v>
+        <v>2.2732878600641099E-3</v>
       </c>
       <c r="F44" s="1">
         <f>PI()* (D44/2)^2</f>
-        <v>7.0685834705770342E-4</v>
+        <v>7.1394460198695691E-4</v>
       </c>
       <c r="G44" s="1">
         <f>E44*B44</f>
-        <v>9.0281518882536686E-4</v>
+        <v>8.638493868243618E-4</v>
       </c>
       <c r="H44" s="1">
         <f>(E44-F44)*B44</f>
-        <v>6.3420901694343954E-4</v>
+        <v>5.9255043806931808E-4</v>
       </c>
       <c r="I44" s="1">
         <f>G44/H44</f>
-        <v>1.4235294117647059</v>
+        <v>1.4578495454986171</v>
       </c>
       <c r="J44" s="1">
         <f>(G44-H44) * 1000</f>
-        <v>0.26860617188192731</v>
+        <v>0.27129894875504373</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1751,50 +1829,347 @@
       </c>
       <c r="G45">
         <f>G44*2</f>
-        <v>1.8056303776507337E-3</v>
+        <v>1.7276987736487236E-3</v>
       </c>
       <c r="H45">
         <f>H44*2</f>
-        <v>1.2684180338868791E-3</v>
+        <v>1.1851008761386362E-3</v>
       </c>
       <c r="I45">
         <f>G45/H45</f>
-        <v>1.4235294117647059</v>
+        <v>1.4578495454986171</v>
       </c>
       <c r="J45" s="1">
         <f>(G45-H45) * 1000</f>
-        <v>0.53721234376385463</v>
+        <v>0.54259789751008747</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="H46" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="C47" s="4">
+      <c r="C47" s="3">
         <v>0.76</v>
       </c>
       <c r="D47" s="3">
         <v>0</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="3">
         <v>0.19</v>
       </c>
       <c r="F47" s="3">
         <v>0.23</v>
+      </c>
+      <c r="H47">
+        <f>(E44-F44)*20684000</f>
+        <v>32253.45595006783</v>
+      </c>
+      <c r="I47">
+        <f>E44*20684000</f>
+        <v>47020.686097566053</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="B50" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3.78E-2</v>
+      </c>
+      <c r="D51" s="2">
+        <f>0.023</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="E51" s="1">
+        <f>PI()* (C51/2)^2</f>
+        <v>1.12220831178881E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>PI()* (D51/2)^2</f>
+        <v>4.154756284372501E-4</v>
+      </c>
+      <c r="G51" s="1">
+        <f>E51*B51</f>
+        <v>1.8179774650978724E-4</v>
+      </c>
+      <c r="H51" s="1">
+        <f>(E51-F51)*B51</f>
+        <v>1.144906947029527E-4</v>
+      </c>
+      <c r="I51" s="1">
+        <f>G51/H51</f>
+        <v>1.5878822901849219</v>
+      </c>
+      <c r="J51" s="1">
+        <f>(G51-H51) * 1000</f>
+        <v>6.7307051806834536E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="G52">
+        <f>G51*2</f>
+        <v>3.6359549301957447E-4</v>
+      </c>
+      <c r="H52">
+        <f>H51*2</f>
+        <v>2.289813894059054E-4</v>
+      </c>
+      <c r="I52">
+        <f>G52/H52</f>
+        <v>1.5878822901849219</v>
+      </c>
+      <c r="J52" s="1">
+        <f>(G52-H52) * 1000</f>
+        <v>0.13461410361366907</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="B53" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" t="s">
+        <v>76</v>
+      </c>
+      <c r="I53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="C54" s="3">
+        <v>-0.14649999999999999</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>-0.14649999999999999</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H54">
+        <f>(E51-F51)*20684000</f>
+        <v>14618.058822443663</v>
+      </c>
+      <c r="I54">
+        <f>E51*20684000</f>
+        <v>23211.756721039746</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="B58" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="C59" s="2">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="D59" s="2">
+        <f>0.035</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E59" s="1">
+        <f>PI()* (C59/2)^2</f>
+        <v>4.9265199356533706E-3</v>
+      </c>
+      <c r="F59" s="1">
+        <f>PI()* (D59/2)^2</f>
+        <v>9.6211275016187424E-4</v>
+      </c>
+      <c r="G59" s="1">
+        <f>E59*B59</f>
+        <v>1.5764863794090786E-3</v>
+      </c>
+      <c r="H59" s="1">
+        <f>(E59-F59)*B59</f>
+        <v>1.2686102993572791E-3</v>
+      </c>
+      <c r="I59" s="1">
+        <f>G59/H59</f>
+        <v>1.242687671862494</v>
+      </c>
+      <c r="J59" s="1">
+        <f>(G59-H59) * 1000</f>
+        <v>0.30787608005179951</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60">
+        <f>G59*2</f>
+        <v>3.1529727588181572E-3</v>
+      </c>
+      <c r="H60">
+        <f>H59*2</f>
+        <v>2.5372205987145582E-3</v>
+      </c>
+      <c r="I60">
+        <f>G60/H60</f>
+        <v>1.242687671862494</v>
+      </c>
+      <c r="J60" s="1">
+        <f>(G60-H60) * 1000</f>
+        <v>0.61575216010359901</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="B61" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" t="s">
+        <v>76</v>
+      </c>
+      <c r="I61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="C62" s="3">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="D62" s="3">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H62">
+        <f>(E59-F59)*20684000</f>
+        <v>81999.798224706115</v>
+      </c>
+      <c r="I62">
+        <f>E59*20684000</f>
+        <v>101900.13834905432</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="C63" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2010,7 +2385,7 @@
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2039,47 +2414,47 @@
       </c>
     </row>
     <row r="35" spans="10:10" ht="15">
-      <c r="J35" s="16" t="s">
+      <c r="J35" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="36" spans="10:10">
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="10:10">
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="38" spans="10:10">
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="39" spans="10:10" ht="22.5">
-      <c r="J39" s="16" t="s">
+      <c r="J39" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="40" spans="10:10">
-      <c r="J40" s="17" t="s">
+      <c r="J40" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="41" spans="10:10" ht="15">
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="10:10">
-      <c r="J42" s="17" t="s">
+      <c r="J42" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="43" spans="10:10" ht="22.5">
-      <c r="J43" s="16" t="s">
+      <c r="J43" s="15" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>